<commit_message>
Excel coords correct this time for real
</commit_message>
<xml_diff>
--- a/Lab 3 MG stuff/Hour and Minute Hand coords.xlsx
+++ b/Lab 3 MG stuff/Hour and Minute Hand coords.xlsx
@@ -389,8 +389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,12 +420,12 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f xml:space="preserve"> ROUND(64 + 33 * COS((PI() / 2) - A2 * (PI() /24)), 0)</f>
+        <f xml:space="preserve"> ROUND(64 + 16 * COS((PI() / 2) - A2 * (PI() /24)), 0)</f>
         <v>64</v>
       </c>
       <c r="C2">
-        <f xml:space="preserve"> ROUND(105 + 33 * SIN((PI() / 2) - A2 * (PI() / 24)),0)</f>
-        <v>138</v>
+        <f xml:space="preserve"> ROUND(105 - 16 * SIN((PI() / 2) - A2 * (PI() / 24)),0)</f>
+        <v>89</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -435,8 +435,8 @@
         <v>64</v>
       </c>
       <c r="G2">
-        <f xml:space="preserve"> ROUND(105 + 33 * SIN((PI() / 2) - E2 * (PI() / 30)),0)</f>
-        <v>138</v>
+        <f xml:space="preserve"> ROUND(105 - 33 * SIN((PI() / 2) - E2 * (PI() / 30)),0)</f>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -444,12 +444,12 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B49" si="0" xml:space="preserve"> ROUND(64 + 33 * COS((PI() / 2) - A3 * (PI() /24)), 0)</f>
-        <v>68</v>
+        <f t="shared" ref="B3:B49" si="0" xml:space="preserve"> ROUND(64 + 16 * COS((PI() / 2) - A3 * (PI() /24)), 0)</f>
+        <v>66</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C49" si="1" xml:space="preserve"> ROUND(105 + 33 * SIN((PI() / 2) - A3 * (PI() / 24)),0)</f>
-        <v>138</v>
+        <f t="shared" ref="C3:C49" si="1" xml:space="preserve"> ROUND(105 - 16 * SIN((PI() / 2) - A3 * (PI() / 24)),0)</f>
+        <v>89</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -459,8 +459,8 @@
         <v>67</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G61" si="3" xml:space="preserve"> ROUND(105 + 33 * SIN((PI() / 2) - E3 * (PI() / 30)),0)</f>
-        <v>138</v>
+        <f t="shared" ref="G3:G61" si="3" xml:space="preserve"> ROUND(105 - 33 * SIN((PI() / 2) - E3 * (PI() / 30)),0)</f>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -469,11 +469,11 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>137</v>
+        <v>90</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -484,7 +484,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="3"/>
-        <v>137</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -493,11 +493,11 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -508,7 +508,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="3"/>
-        <v>136</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -517,11 +517,11 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -532,7 +532,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="3"/>
-        <v>135</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -541,11 +541,11 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -556,7 +556,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="3"/>
-        <v>134</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -565,11 +565,11 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -580,7 +580,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="3"/>
-        <v>132</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -589,11 +589,11 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -604,7 +604,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="3"/>
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -613,11 +613,11 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -628,7 +628,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="3"/>
-        <v>127</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -637,11 +637,11 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="E11">
         <v>9</v>
@@ -652,7 +652,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
-        <v>124</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -661,11 +661,11 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -676,7 +676,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="3"/>
-        <v>122</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -685,11 +685,11 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E13">
         <v>11</v>
@@ -700,7 +700,7 @@
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
-        <v>118</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -709,7 +709,7 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
@@ -724,7 +724,7 @@
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -733,11 +733,11 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E15">
         <v>13</v>
@@ -748,7 +748,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="3"/>
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -757,11 +757,11 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="E16">
         <v>14</v>
@@ -772,7 +772,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="3"/>
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -781,11 +781,11 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="E17">
         <v>15</v>
@@ -805,11 +805,11 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -820,7 +820,7 @@
       </c>
       <c r="G18">
         <f t="shared" si="3"/>
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -829,11 +829,11 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="E19">
         <v>17</v>
@@ -844,7 +844,7 @@
       </c>
       <c r="G19">
         <f t="shared" si="3"/>
-        <v>98</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -853,11 +853,11 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="E20">
         <v>18</v>
@@ -868,7 +868,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -877,11 +877,11 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="E21">
         <v>19</v>
@@ -892,7 +892,7 @@
       </c>
       <c r="G21">
         <f t="shared" si="3"/>
-        <v>92</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -901,11 +901,11 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="E22">
         <v>20</v>
@@ -916,7 +916,7 @@
       </c>
       <c r="G22">
         <f t="shared" si="3"/>
-        <v>89</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -925,11 +925,11 @@
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="E23">
         <v>21</v>
@@ -940,7 +940,7 @@
       </c>
       <c r="G23">
         <f t="shared" si="3"/>
-        <v>86</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -949,11 +949,11 @@
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E24">
         <v>22</v>
@@ -964,7 +964,7 @@
       </c>
       <c r="G24">
         <f t="shared" si="3"/>
-        <v>83</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -973,11 +973,11 @@
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="E25">
         <v>23</v>
@@ -988,7 +988,7 @@
       </c>
       <c r="G25">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="E26">
         <v>24</v>
@@ -1012,7 +1012,7 @@
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>78</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1021,11 +1021,11 @@
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="E27">
         <v>25</v>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="G27">
         <f t="shared" si="3"/>
-        <v>76</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1045,11 +1045,11 @@
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="E28">
         <v>26</v>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="G28">
         <f t="shared" si="3"/>
-        <v>75</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1069,11 +1069,11 @@
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="E29">
         <v>27</v>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="G29">
         <f t="shared" si="3"/>
-        <v>74</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1093,11 +1093,11 @@
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="E30">
         <v>28</v>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="G30">
         <f t="shared" si="3"/>
-        <v>73</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1117,11 +1117,11 @@
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="E31">
         <v>29</v>
@@ -1132,7 +1132,7 @@
       </c>
       <c r="G31">
         <f t="shared" si="3"/>
-        <v>72</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1141,11 +1141,11 @@
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="E32">
         <v>30</v>
@@ -1156,7 +1156,7 @@
       </c>
       <c r="G32">
         <f t="shared" si="3"/>
-        <v>72</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1165,11 +1165,11 @@
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="E33">
         <v>31</v>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="G33">
         <f t="shared" si="3"/>
-        <v>72</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1189,11 +1189,11 @@
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="E34">
         <v>32</v>
@@ -1204,7 +1204,7 @@
       </c>
       <c r="G34">
         <f t="shared" si="3"/>
-        <v>73</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1213,11 +1213,11 @@
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="E35">
         <v>33</v>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="G35">
         <f t="shared" si="3"/>
-        <v>74</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1237,11 +1237,11 @@
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="E36">
         <v>34</v>
@@ -1252,7 +1252,7 @@
       </c>
       <c r="G36">
         <f t="shared" si="3"/>
-        <v>75</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1261,11 +1261,11 @@
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E37">
         <v>35</v>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="G37">
         <f t="shared" si="3"/>
-        <v>76</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
@@ -1300,7 +1300,7 @@
       </c>
       <c r="G38">
         <f t="shared" si="3"/>
-        <v>78</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1309,11 +1309,11 @@
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E39">
         <v>37</v>
@@ -1324,7 +1324,7 @@
       </c>
       <c r="G39">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1333,11 +1333,11 @@
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E40">
         <v>38</v>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="G40">
         <f t="shared" si="3"/>
-        <v>83</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1357,11 +1357,11 @@
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="E41">
         <v>39</v>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="G41">
         <f t="shared" si="3"/>
-        <v>86</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1381,11 +1381,11 @@
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="G42">
         <f t="shared" si="3"/>
-        <v>89</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1405,11 +1405,11 @@
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="E43">
         <v>41</v>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="G43">
         <f t="shared" si="3"/>
-        <v>92</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1429,11 +1429,11 @@
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="E44">
         <v>42</v>
@@ -1444,7 +1444,7 @@
       </c>
       <c r="G44">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1453,11 +1453,11 @@
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="E45">
         <v>43</v>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="G45">
         <f t="shared" si="3"/>
-        <v>98</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1477,11 +1477,11 @@
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="E46">
         <v>44</v>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="G46">
         <f t="shared" si="3"/>
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1501,11 +1501,11 @@
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="E47">
         <v>45</v>
@@ -1525,11 +1525,11 @@
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
-        <v>137</v>
+        <v>90</v>
       </c>
       <c r="E48">
         <v>46</v>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="G48">
         <f t="shared" si="3"/>
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1549,11 +1549,11 @@
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
-        <v>138</v>
+        <v>89</v>
       </c>
       <c r="E49">
         <v>47</v>
@@ -1564,7 +1564,7 @@
       </c>
       <c r="G49">
         <f t="shared" si="3"/>
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="G50">
         <f t="shared" si="3"/>
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -1590,7 +1590,7 @@
       </c>
       <c r="G51">
         <f t="shared" si="3"/>
-        <v>118</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="G52">
         <f t="shared" si="3"/>
-        <v>122</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="G53">
         <f t="shared" si="3"/>
-        <v>124</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="G54">
         <f t="shared" si="3"/>
-        <v>127</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1642,7 +1642,7 @@
       </c>
       <c r="G55">
         <f t="shared" si="3"/>
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -1655,7 +1655,7 @@
       </c>
       <c r="G56">
         <f t="shared" si="3"/>
-        <v>132</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1668,7 +1668,7 @@
       </c>
       <c r="G57">
         <f t="shared" si="3"/>
-        <v>134</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="G58">
         <f t="shared" si="3"/>
-        <v>135</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="G59">
         <f t="shared" si="3"/>
-        <v>136</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="G60">
         <f t="shared" si="3"/>
-        <v>137</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="G61">
         <f t="shared" si="3"/>
-        <v>138</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>